<commit_message>
first onClickOption and Customer
</commit_message>
<xml_diff>
--- a/P06/Scrum_Sprint_2.xlsx
+++ b/P06/Scrum_Sprint_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcnar\Desktop\cse1325\P06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1C14B7-F0BC-4EC7-A4D4-C24B21118086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A0B943-E3D7-417A-9969-0DDDF396E694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5655" yWindow="2985" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="194">
   <si>
     <t>Product Name:</t>
   </si>
@@ -609,6 +609,21 @@
   </si>
   <si>
     <t>Finished in Sprint 2</t>
+  </si>
+  <si>
+    <t>Begin constructing the onInsertCustomerClick()</t>
+  </si>
+  <si>
+    <t>Test onInsertCustomerClick() using gui only</t>
+  </si>
+  <si>
+    <t>Begin constructing the onInsertOptionClick()</t>
+  </si>
+  <si>
+    <t>test onInsertOptionClick() using gui only</t>
+  </si>
+  <si>
+    <t>Git add, commit, push</t>
   </si>
 </sst>
 </file>
@@ -898,6 +913,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -912,12 +933,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1144,16 +1159,16 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1438,10 +1453,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3815,7 +3830,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3838,14 +3853,14 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="47" t="s">
         <v>154</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
       <c r="H1" s="5"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
@@ -3856,14 +3871,14 @@
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="48" t="s">
         <v>153</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -3902,14 +3917,14 @@
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="49" t="s">
         <v>155</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
       <c r="H5" s="3" t="s">
         <v>156</v>
       </c>
@@ -3920,48 +3935,48 @@
     </row>
     <row r="6" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="5"/>
@@ -4049,11 +4064,11 @@
       </c>
       <c r="B14" s="5">
         <f>B13-C14</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 2")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="5"/>
@@ -4073,7 +4088,7 @@
       </c>
       <c r="B15" s="5">
         <f>B14-C15</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 3")</f>
@@ -4097,7 +4112,7 @@
       </c>
       <c r="B16" s="5">
         <f>B15-C16</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 4")</f>
@@ -4117,7 +4132,7 @@
       </c>
       <c r="B17" s="5">
         <f>B16-C17</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 4")</f>
@@ -4189,10 +4204,10 @@
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
-      <c r="F22" s="44" t="s">
+      <c r="F22" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="44"/>
+      <c r="G22" s="46"/>
       <c r="H22" s="13"/>
       <c r="I22" s="13" t="s">
         <v>19</v>
@@ -4443,7 +4458,9 @@
       <c r="F30" s="17">
         <v>2</v>
       </c>
-      <c r="G30" s="17"/>
+      <c r="G30" s="17" t="s">
+        <v>188</v>
+      </c>
       <c r="H30" s="18" t="s">
         <v>31</v>
       </c>
@@ -5759,7 +5776,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5864,7 +5881,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -5879,7 +5896,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -5901,7 +5918,7 @@
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
@@ -6039,7 +6056,7 @@
       <c r="C17" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D17" s="49" t="s">
+      <c r="D17" s="44" t="s">
         <v>184</v>
       </c>
       <c r="E17" s="37" t="s">
@@ -6115,60 +6132,108 @@
       <c r="A22" s="4">
         <v>6</v>
       </c>
-      <c r="B22" s="35"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="37"/>
+      <c r="B22" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D22" s="39" t="s">
+        <v>189</v>
+      </c>
+      <c r="E22" s="37" t="s">
+        <v>173</v>
+      </c>
       <c r="F22" s="38"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>7</v>
       </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="37"/>
+      <c r="B23" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D23" s="39" t="s">
+        <v>190</v>
+      </c>
+      <c r="E23" s="37" t="s">
+        <v>173</v>
+      </c>
       <c r="F23" s="38"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>8</v>
       </c>
-      <c r="B24" s="35"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="37"/>
+      <c r="B24" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D24" s="39" t="s">
+        <v>193</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>173</v>
+      </c>
       <c r="F24" s="38"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>9</v>
       </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="37"/>
+      <c r="B25" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D25" s="39" t="s">
+        <v>191</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>173</v>
+      </c>
       <c r="F25" s="38"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>10</v>
       </c>
-      <c r="B26" s="35"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="37"/>
+      <c r="B26" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D26" s="39" t="s">
+        <v>192</v>
+      </c>
+      <c r="E26" s="37" t="s">
+        <v>173</v>
+      </c>
       <c r="F26" s="38"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>11</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="37"/>
+      <c r="B27" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D27" s="39" t="s">
+        <v>193</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>173</v>
+      </c>
       <c r="F27" s="38"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -7237,7 +7302,7 @@
       <c r="C17" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D17" s="48" t="s">
+      <c r="D17" s="43" t="s">
         <v>157</v>
       </c>
       <c r="E17" s="37" t="s">

</xml_diff>

<commit_message>
Still working on onClickComputer()
</commit_message>
<xml_diff>
--- a/P06/Scrum_Sprint_2.xlsx
+++ b/P06/Scrum_Sprint_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcnar\Desktop\cse1325\P06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A0B943-E3D7-417A-9969-0DDDF396E694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595E6C7C-3D80-4F24-A210-95FF25CE26E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7080" yWindow="2820" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="197">
   <si>
     <t>Product Name:</t>
   </si>
@@ -624,6 +624,15 @@
   </si>
   <si>
     <t>Git add, commit, push</t>
+  </si>
+  <si>
+    <t>Construct onInsertComputerClick()</t>
+  </si>
+  <si>
+    <t>test with gui only</t>
+  </si>
+  <si>
+    <t>In Work</t>
   </si>
 </sst>
 </file>
@@ -1159,16 +1168,16 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1453,28 +1462,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3829,8 +3838,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4064,11 +4073,11 @@
       </c>
       <c r="B14" s="5">
         <f>B13-C14</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 2")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="5"/>
@@ -4088,7 +4097,7 @@
       </c>
       <c r="B15" s="5">
         <f>B14-C15</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 3")</f>
@@ -4112,7 +4121,7 @@
       </c>
       <c r="B16" s="5">
         <f>B15-C16</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 4")</f>
@@ -4132,7 +4141,7 @@
       </c>
       <c r="B17" s="5">
         <f>B16-C17</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 4")</f>
@@ -4491,7 +4500,9 @@
       <c r="F31" s="17">
         <v>2</v>
       </c>
-      <c r="G31" s="17"/>
+      <c r="G31" s="17" t="s">
+        <v>188</v>
+      </c>
       <c r="H31" s="18" t="s">
         <v>31</v>
       </c>
@@ -5775,8 +5786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A21" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5881,7 +5892,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -5896,7 +5907,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -5914,7 +5925,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -5932,7 +5943,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -5950,7 +5961,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -5968,7 +5979,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -5986,7 +5997,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -6004,7 +6015,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -6250,30 +6261,54 @@
       <c r="A29" s="4">
         <v>13</v>
       </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="37"/>
+      <c r="B29" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D29" s="39" t="s">
+        <v>194</v>
+      </c>
+      <c r="E29" s="37" t="s">
+        <v>196</v>
+      </c>
       <c r="F29" s="38"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>14</v>
       </c>
-      <c r="B30" s="35"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="37"/>
+      <c r="B30" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D30" s="39" t="s">
+        <v>195</v>
+      </c>
+      <c r="E30" s="37" t="s">
+        <v>196</v>
+      </c>
       <c r="F30" s="38"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>15</v>
       </c>
-      <c r="B31" s="35"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="37"/>
+      <c r="B31" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D31" s="39" t="s">
+        <v>193</v>
+      </c>
+      <c r="E31" s="37" t="s">
+        <v>196</v>
+      </c>
       <c r="F31" s="38"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
still working on onViewClick()
</commit_message>
<xml_diff>
--- a/P06/Scrum_Sprint_2.xlsx
+++ b/P06/Scrum_Sprint_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcnar\Desktop\cse1325\P06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD06EAFB-AB5A-45EE-A7E0-10BFCA28FA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E5C913-5FED-457C-B395-C1CE40DD2073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="200">
   <si>
     <t>Product Name:</t>
   </si>
@@ -636,6 +636,12 @@
   </si>
   <si>
     <t>Completed Day 3</t>
+  </si>
+  <si>
+    <t>In Work</t>
+  </si>
+  <si>
+    <t>Construct onViewClick() method</t>
   </si>
 </sst>
 </file>
@@ -1465,28 +1471,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3841,8 +3847,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4566,7 +4572,7 @@
         <v>2</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="H33" s="18" t="s">
         <v>31</v>
@@ -5795,8 +5801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="E21" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView topLeftCell="A21" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5901,7 +5907,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -5916,7 +5922,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -5934,7 +5940,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -5952,7 +5958,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -5970,7 +5976,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -5988,7 +5994,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -6006,7 +6012,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -6024,7 +6030,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -6334,10 +6340,18 @@
       <c r="A33" s="4">
         <v>17</v>
       </c>
-      <c r="B33" s="35"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="37"/>
+      <c r="B33" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D33" s="39" t="s">
+        <v>199</v>
+      </c>
+      <c r="E33" s="37" t="s">
+        <v>198</v>
+      </c>
       <c r="F33" s="38"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -6346,8 +6360,12 @@
       </c>
       <c r="B34" s="35"/>
       <c r="C34" s="4"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="37"/>
+      <c r="D34" s="39" t="s">
+        <v>195</v>
+      </c>
+      <c r="E34" s="37" t="s">
+        <v>198</v>
+      </c>
       <c r="F34" s="38"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -6356,8 +6374,12 @@
       </c>
       <c r="B35" s="35"/>
       <c r="C35" s="4"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="37"/>
+      <c r="D35" s="39" t="s">
+        <v>193</v>
+      </c>
+      <c r="E35" s="37" t="s">
+        <v>198</v>
+      </c>
       <c r="F35" s="38"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>